<commit_message>
removed unused dt and dx parameters in favour of the higher level number of timesteps given from excel parameter sheet through the produce family raster function
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,12 +22,83 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Dt = 1day/timestep;
+I.e., number of timesteps per day. For instance, a value of 24 means that dt=1 hour.
+ </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Used as alternative timestep when normal_timestep doesnt converge</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres. Only used if rectangular grid
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t xml:space="preserve">NDAYS</t>
   </si>
   <si>
+    <t xml:space="preserve">normal_timestep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shorter_timestep</t>
+  </si>
+  <si>
     <t xml:space="preserve">number</t>
   </si>
   <si>
@@ -65,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">channel_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dx</t>
   </si>
   <si>
     <t xml:space="preserve">porous_threshold</t>
@@ -146,7 +220,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,7 +230,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFDEEBF7"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
     <fill>
@@ -189,6 +263,12 @@
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
@@ -224,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,6 +334,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,7 +361,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFE7E6E6"/>
+      <rgbColor rgb="FFEEEEEE"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -309,7 +393,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE7E6E6"/>
       <rgbColor rgb="FFE2F0D9"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -342,22 +426,38 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>364</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -368,6 +468,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -382,26 +483,26 @@
       <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,102 +657,109 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="D2" s="9"/>
       <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="H2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="9" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2" s="6" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="10" t="n">
         <v>1.5</v>
       </c>
-      <c r="J2" s="9" t="n">
+      <c r="K2" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="M2" s="10" t="n">
         <v>1000</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="N2" s="8" t="n">
         <v>100000</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="O2" s="8" t="n">
         <v>50</v>
       </c>
     </row>
@@ -671,38 +779,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.35"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1000</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -713,5 +827,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added comments to understand parameters
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,6 +28,20 @@
     <author> </author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Outermost loop. Number of days to simulate. </t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B1" authorId="0">
       <text>
         <r>
@@ -54,7 +68,256 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Used as alternative timestep when normal_timestep doesnt converge</t>
+          <t xml:space="preserve">Used as a fallback value   when normal_timestep doesnt converge.
+It serves as a very rough but performant adaptive timestep solution to the convergence problems of the hydrology model .</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This is the number to reference from the code (and not the excel column numbers!)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">See parameterizations for the specific yield and transmissivity functions</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+A value of 0 means that the highest point of the block (aka ‘block head’) is level with the adjacent peat.
+A value of -0.3 would mean that  the block head is 30 cm below </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">the adjacent peat.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">SI units.
+Used to compute the amount of water flow through the blocks.  See paper.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+Initial value for the CWL at canals, relative to the peat surface height (DEM).
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">m^3/s
+Initial value for the discharge. Only used when solving with the Preissmann scheme.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+Depth of channel bed.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">We don’t have measurements of the slope of the channel bed and so we assume that the channel bed is parallel to the peat surface.
+The CWL can never go below this value, or otherwise a numerical error occurs. Therefore, this value should always be large. 8 metres has always been fine. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+CWL boundary conditions at the  downstream and/or upstream  nodes of each channel reach.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">m³/s
+Dirichlet BC for the water discharge. Only used for the Preissmann scheme</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+Width of the channels.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Metres.
+Distance between nodes of the channel network.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Parameters used to describe the Manning friction term in the open channel flow equations</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Maximum number of iterations to avoid infinite loops in the Newton method computation step</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Analogous quantity for the inexact fo accelerated Newton method. 
+The inexact newton method needs less computations of the jacobian, and, for that reason, it is usually more efficient</t>
         </r>
       </text>
     </comment>
@@ -78,7 +341,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Use only if boundary_condition=’dirichlet’.
+          <t xml:space="preserve">Meters.
+Used only if boundary_condition=’dirichlet’.
 Else, if boundary_condition=’neumann’, this value will be ignored and Neumann boundary conditions applied
 </t>
         </r>
@@ -94,7 +358,8 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Metres. Only used if rectangular grid
+          <t xml:space="preserve">Metres.
+Only used if rectangular grid hydrology
 </t>
         </r>
       </text>
@@ -212,7 +477,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -234,6 +499,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -448,7 +719,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
@@ -496,10 +767,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
   </cols>
@@ -665,6 +936,7 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -675,16 +947,19 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="24.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -744,7 +1019,9 @@
       <c r="C2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="9" t="n">
+        <v>0</v>
+      </c>
       <c r="E2" s="6" t="s">
         <v>26</v>
       </c>
@@ -787,6 +1064,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -797,11 +1075,11 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.35"/>

</xml_diff>